<commit_message>
Remove temporary Excel files
</commit_message>
<xml_diff>
--- a/data/providers_data.xlsx
+++ b/data/providers_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\food-wastage-system\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CF43E18-B1C4-4B41-9E1D-1F4453CB96D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFABE10-CD88-4596-BD9F-B0006CB41664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7361704C-6E65-46E4-9A95-10A50FDB3A2D}"/>
   </bookViews>
@@ -12909,11 +12909,12 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.109375" bestFit="1" customWidth="1"/>

</xml_diff>